<commit_message>
Change hour format to 12 hours
</commit_message>
<xml_diff>
--- a/Metodos Cuantitativos/Act 8 - Fila de espera con un servidor/output.xlsx
+++ b/Metodos Cuantitativos/Act 8 - Fila de espera con un servidor/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8vo Semestre\Aplicaciones Avanzadas\TC3002B_Development-of-Advanced-Applications-of-Computer-Science\Metodos Cuantitativos\Act 8 - Fila de espera con un servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3099E9-9986-472B-923E-75F451A0FDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FC0031-CF28-44FD-BEF4-CDAB98D1A1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Cliente</t>
   </si>
@@ -44,15 +44,126 @@
   </si>
   <si>
     <t>Tiempo inactividad del ATM</t>
+  </si>
+  <si>
+    <t>06:00 PM</t>
+  </si>
+  <si>
+    <t>06:02 PM</t>
+  </si>
+  <si>
+    <t>06:10 PM</t>
+  </si>
+  <si>
+    <t>06:14 PM</t>
+  </si>
+  <si>
+    <t>06:17 PM</t>
+  </si>
+  <si>
+    <t>06:22 PM</t>
+  </si>
+  <si>
+    <t>06:26 PM</t>
+  </si>
+  <si>
+    <t>06:29 PM</t>
+  </si>
+  <si>
+    <t>06:28 PM</t>
+  </si>
+  <si>
+    <t>06:32 PM</t>
+  </si>
+  <si>
+    <t>06:35 PM</t>
+  </si>
+  <si>
+    <t>06:37 PM</t>
+  </si>
+  <si>
+    <t>06:39 PM</t>
+  </si>
+  <si>
+    <t>06:46 PM</t>
+  </si>
+  <si>
+    <t>06:51 PM</t>
+  </si>
+  <si>
+    <t>06:53 PM</t>
+  </si>
+  <si>
+    <t>06:55 PM</t>
+  </si>
+  <si>
+    <t>06:59 PM</t>
+  </si>
+  <si>
+    <t>07:01 PM</t>
+  </si>
+  <si>
+    <t>07:03 PM</t>
+  </si>
+  <si>
+    <t>07:04 PM</t>
+  </si>
+  <si>
+    <t>07:08 PM</t>
+  </si>
+  <si>
+    <t>07:11 PM</t>
+  </si>
+  <si>
+    <t>07:13 PM</t>
+  </si>
+  <si>
+    <t>07:18 PM</t>
+  </si>
+  <si>
+    <t>07:22 PM</t>
+  </si>
+  <si>
+    <t>07:19 PM</t>
+  </si>
+  <si>
+    <t>07:27 PM</t>
+  </si>
+  <si>
+    <t>07:25 PM</t>
+  </si>
+  <si>
+    <t>07:30 PM</t>
+  </si>
+  <si>
+    <t>07:34 PM</t>
+  </si>
+  <si>
+    <t>07:35 PM</t>
+  </si>
+  <si>
+    <t>07:41 PM</t>
+  </si>
+  <si>
+    <t>07:42 PM</t>
+  </si>
+  <si>
+    <t>07:45 PM</t>
+  </si>
+  <si>
+    <t>07:46 PM</t>
+  </si>
+  <si>
+    <t>07:49 PM</t>
+  </si>
+  <si>
+    <t>07:50 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,12 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,18 +520,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -459,17 +570,17 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.375</v>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.375</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.377777777777778</v>
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -483,25 +594,25 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.375694444444445</v>
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.377777777777778</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.377777777777778</v>
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -509,25 +620,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.377083333333333</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.377777777777778</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.3791666666666671</v>
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -535,25 +646,25 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.377083333333333</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
-        <v>1.3791666666666671</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.3812500000000001</v>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -561,25 +672,25 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.3833333333333331</v>
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.3833333333333331</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.3861111111111111</v>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -589,17 +700,17 @@
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.388194444444445</v>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.388194444444445</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.3888888888888891</v>
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -613,25 +724,25 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.39375</v>
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="2">
-        <v>1.39375</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.3951388888888889</v>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -639,25 +750,25 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.3951388888888889</v>
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.3951388888888889</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.3951388888888889</v>
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -665,25 +776,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.3951388888888889</v>
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.3951388888888889</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.395833333333333</v>
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -691,25 +802,285 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.398611111111111</v>
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1.398611111111111</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1.400694444444444</v>
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>